<commit_message>
[Manager] - finish ; Add logback
</commit_message>
<xml_diff>
--- a/Database/table-spec.xlsx
+++ b/Database/table-spec.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank\Desktop\Chatroom\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC2E2C4-7B07-4465-A60E-9B0BEF5B8F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC8820E-07B6-4B7B-89D3-61465CF2B3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="會員" sheetId="1" r:id="rId1"/>
     <sheet name="好友" sheetId="3" r:id="rId2"/>
+    <sheet name="管理員" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>表格名稱</t>
   </si>
@@ -70,9 +71,6 @@
     <t>PK,AI</t>
   </si>
   <si>
-    <t>VARCHAR</t>
-  </si>
-  <si>
     <t>NOT NULL</t>
   </si>
   <si>
@@ -97,12 +95,6 @@
     <t>照片</t>
   </si>
   <si>
-    <t>BLOB</t>
-  </si>
-  <si>
-    <t>TINYINT</t>
-  </si>
-  <si>
     <t>會員狀態</t>
   </si>
   <si>
@@ -115,10 +107,6 @@
   </si>
   <si>
     <t>LOGIN_STATUS</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>TINYINT</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -275,6 +263,85 @@
 0: 待確認
 1: 已確認
 2: 已取消</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>性別</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL
+0: 女
+1: 男</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>GENDER</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理員</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANAGER</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MANAGER_ID</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理員編號</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>帳號</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>密碼</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>權限</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOT NULL
+Admin, Manager</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROLE</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACCOUT</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATE</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -352,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -740,18 +807,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF4F4F4F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF4F4F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF432706"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF4F4F4F"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF4F4F4F"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF4F4F4F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF432706"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF4F4F4F"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF4F4F4F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF4F4F4F"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF432706"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF4F4F4F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF432706"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF4F4F4F"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -764,14 +941,116 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -779,88 +1058,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -1141,279 +1359,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.09765625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.796875" style="9"/>
+    <col min="1" max="1" width="9.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.09765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.3984375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="54"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="24">
+        <v>1</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="A6" s="24">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="11">
+        <v>50</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="11">
+        <v>50</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="24">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="11">
+        <v>255</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39.5" thickBot="1">
+      <c r="A9" s="24">
+        <v>5</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1">
+      <c r="A10" s="24">
+        <v>6</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="11">
+        <v>10</v>
+      </c>
+      <c r="F10" s="14"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1">
+      <c r="A11" s="24">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1">
+      <c r="A12" s="24">
+        <v>8</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="11">
+        <v>255</v>
+      </c>
+      <c r="F12" s="61"/>
+    </row>
+    <row r="13" spans="1:6" ht="39.5" thickBot="1">
+      <c r="A13" s="24">
+        <v>9</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="59">
+        <v>1</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+    </row>
+    <row r="14" spans="1:6" ht="52.5" thickBot="1">
+      <c r="A14" s="24">
+        <v>10</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="26">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
-      <c r="A5" s="41">
-        <v>1</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="F14" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1">
+      <c r="A15" s="24">
         <v>11</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="B15" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1">
+      <c r="A16" s="24">
         <v>12</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
-      <c r="A6" s="41">
-        <v>2</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="25">
-        <v>50</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
-      <c r="A7" s="41">
-        <v>3</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="25">
-        <v>255</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1">
-      <c r="A8" s="41">
-        <v>4</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="25">
-        <v>50</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
-      <c r="A9" s="41">
-        <v>5</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="25">
-        <v>10</v>
-      </c>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="41">
-        <v>6</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="25" t="s">
+      <c r="B16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1">
-      <c r="A11" s="41">
-        <v>7</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
-    </row>
-    <row r="12" spans="1:6" ht="39.5" thickBot="1">
-      <c r="A12" s="41">
-        <v>8</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="40" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="52.5" thickBot="1">
-      <c r="A13" s="41">
-        <v>9</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="42" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1">
-      <c r="A14" s="41">
-        <v>10</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1">
-      <c r="A15" s="41">
-        <v>11</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="30" t="s">
+      <c r="E16" s="17"/>
+      <c r="F16" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="42" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1437,7 +1681,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.59765625" defaultRowHeight="14.5"/>
@@ -1446,177 +1690,400 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="56"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="58"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="24">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="A6" s="24">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="11">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="24">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="11">
+        <v>10</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="52.5" thickBot="1">
+      <c r="A8" s="24">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1">
+      <c r="A9" s="24">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D9" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1">
+      <c r="A10" s="24">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B98481-ACCE-482D-AC82-B75DFC8F3513}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.59765625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A2" s="10" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1">
+      <c r="A2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="58"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1">
+      <c r="A5" s="24">
+        <v>1</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1">
+      <c r="A6" s="24">
+        <v>2</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="11">
+        <v>30</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1">
+      <c r="A7" s="32">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="11">
+        <v>30</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1">
+      <c r="A8" s="22">
+        <v>4</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="18">
+        <v>30</v>
+      </c>
+      <c r="F8" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="26.5" thickBot="1">
+      <c r="A9" s="22">
+        <v>5</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="20">
+        <v>30</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1">
+      <c r="A10" s="22">
+        <v>6</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1">
+      <c r="A11" s="22">
+        <v>7</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="46"/>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1">
-      <c r="A4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1">
-      <c r="A5" s="41">
-        <v>1</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" thickBot="1">
-      <c r="A6" s="41">
-        <v>2</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="25">
-        <v>10</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1">
-      <c r="A7" s="41">
-        <v>3</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="25">
-        <v>10</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="52.5" thickBot="1">
-      <c r="A8" s="41">
-        <v>4</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" thickBot="1">
-      <c r="A9" s="41">
-        <v>5</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="40" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" thickBot="1">
-      <c r="A10" s="41">
-        <v>6</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="30" t="s">
+      <c r="D11" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="42" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>